<commit_message>
1. Termin Pembayaran perbulan 2. Kwitansi Angsuran ada bulan dalam format string
</commit_message>
<xml_diff>
--- a/Documents/Backlog.xlsx
+++ b/Documents/Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>Asli Motor</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>Suku Bunga (%)</t>
-  </si>
-  <si>
-    <t>Check lagi</t>
   </si>
 </sst>
 </file>
@@ -496,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B12" activeCellId="1" sqref="B8 B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -508,13 +505,13 @@
     <col min="2" max="2" width="62.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -525,7 +522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -536,7 +533,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -547,7 +544,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -558,7 +555,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>4</v>
       </c>
@@ -566,15 +563,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>6</v>
       </c>
@@ -585,7 +585,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>7</v>
       </c>
@@ -593,7 +593,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>8</v>
       </c>
@@ -604,7 +604,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>9</v>
       </c>
@@ -614,11 +614,8 @@
       <c r="C12" t="s">
         <v>13</v>
       </c>
-      <c r="D12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>10</v>
       </c>
@@ -629,17 +626,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>13</v>
       </c>
@@ -678,7 +675,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -708,7 +705,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>90</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -717,7 +714,7 @@
       </c>
       <c r="B5" s="4">
         <f>(B3*30)/B4</f>
-        <v>12</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -793,19 +790,19 @@
       </c>
       <c r="B17" s="6">
         <f>ROUND((C14+C16)/B5, -3)</f>
-        <v>1688000</v>
+        <v>563000</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="B18" s="2">
         <f>B17*36</f>
-        <v>60768000</v>
+        <v>20268000</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="B19" s="2">
         <f>B18-B17</f>
-        <v>59080000</v>
+        <v>19705000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>